<commit_message>
Correción de errores de campos
</commit_message>
<xml_diff>
--- a/Taller/build/classes/input_file/Tabla.xlsx
+++ b/Taller/build/classes/input_file/Tabla.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A903CE-A352-4155-9078-1E0077D9BDF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02448F6C-56CD-4A57-A271-F295347243F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,10 +46,10 @@
     <t>luque</t>
   </si>
   <si>
-    <t>Edad</t>
-  </si>
-  <si>
     <t>Nataly</t>
+  </si>
+  <si>
+    <t>Edada1</t>
   </si>
 </sst>
 </file>
@@ -377,76 +377,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F5"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="C2">
         <v>25</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="C3">
         <v>26</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4">
+      <c r="C4">
         <v>27</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
       <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5">
+      <c r="C5">
         <v>28</v>
       </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>